<commit_message>
Rehashing the kinetic data (no changes), draft updates through section 3.1.4
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaCaMont_pH7/RaCaMont_pH7_Kinetics_NoScript.xlsx
+++ b/Sorption Experiments/RaCaMont_pH7/RaCaMont_pH7_Kinetics_NoScript.xlsx
@@ -684,7 +684,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -804,11 +803,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="377683808"/>
-        <c:axId val="377684984"/>
+        <c:axId val="489594152"/>
+        <c:axId val="489594544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="377683808"/>
+        <c:axId val="489594152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -865,12 +864,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377684984"/>
+        <c:crossAx val="489594544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="377684984"/>
+        <c:axId val="489594544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -927,7 +926,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377683808"/>
+        <c:crossAx val="489594152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1934,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3775,7 +3774,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4294,7 +4293,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4713,10 +4712,10 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O20" sqref="O20"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>